<commit_message>
cleaned up some slop and added readme
</commit_message>
<xml_diff>
--- a/data/growth_curves.xlsx
+++ b/data/growth_curves.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alex\projects\harvest-timing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5358D062-450B-4BC3-AACB-9463EB0FF286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C449CD81-BA25-4BA4-A391-82C1B4EC5DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57490" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carbon table" sheetId="1" r:id="rId1"/>
     <sheet name="price_over_time" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'carbon table'!$H$2:$H$3</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'carbon table'!$L$2:$L$3</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">price_over_time!$F$2:$F$5</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
@@ -45,7 +45,7 @@
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'carbon table'!$H$5</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'carbon table'!$L$5</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">price_over_time!$F$7</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Age</t>
   </si>
@@ -160,15 +160,27 @@
   <si>
     <t>Recovered %</t>
   </si>
+  <si>
+    <t>Actual stock (harvest at 28 with 10-year decay) no replant</t>
+  </si>
+  <si>
+    <t>Stock change</t>
+  </si>
+  <si>
+    <t>Averaging</t>
+  </si>
+  <si>
+    <t>Permanent</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,12 +194,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -231,19 +237,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +513,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'carbon table'!$E$1</c:f>
+              <c:f>'carbon table'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -535,7 +536,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'carbon table'!$E$2:$E$52</c:f>
+              <c:f>'carbon table'!$I$2:$I$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -958,6 +959,897 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>'carbon table'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stock change</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'carbon table'!$E$2:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35570308063309297</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>144.32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>182.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>220.88</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>259.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>292.16000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>328.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>366.96</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>408.32</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>449.68</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>535.91999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>579.04</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>622.16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>664.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>706.64</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>789.36</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>830.72</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>871.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>911.68</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>951.28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>447.92</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>403.48370308063312</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>360.096</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>318.82399999999996</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>291.63199999999995</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>276.75999999999993</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>275.96799999999996</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>278.69599999999991</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>271.74399999999991</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>265.67199999999991</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>259.59999999999997</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>292.16000000000003</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>328.24</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>366.96</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>408.32</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>449.68</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>535.91999999999996</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>579.04</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>622.16</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>664.4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>706.64</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>748</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F13F-408B-9CAA-C76A30A403A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'carbon table'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Averaging</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'carbon table'!$F$2:$F$52</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35570308063309297</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>144.32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>182.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>220.88</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>259.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>292.16000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>328.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>366.96</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>408.32</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>449.68</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>492.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F13F-408B-9CAA-C76A30A403A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'carbon table'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Permanent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'carbon table'!$G$2:$G$52</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35570308063309297</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>144.32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>182.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>220.88</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>259.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>292.16000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>328.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>366.96</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>408.32</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>449.68</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>492.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>535.91999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>579.04</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>622.16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>664.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>706.64</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>789.36</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>830.72</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>871.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>911.68</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>951.28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>990.88</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1028.72</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1066.56</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1103.52</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1139.5999999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1173.92</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1208.24</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1241.68</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1273.3599999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1305.04</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1336.72</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1366.64</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1396.56</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1426.48</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1455.52</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1483.68</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1510.96</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1537.36</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1562.88</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1588.4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1612.16</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1636.8</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1659.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F13F-408B-9CAA-C76A30A403A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1946358656"/>
+        <c:axId val="1946355296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1946358656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1946355296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1946355296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>NZU accumulation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1946358656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>price_over_time!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1658,7 +2550,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1963,7 +2855,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2428,6 +3320,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3461,6 +4393,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3976,7 +5424,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4496,13 +5944,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>22224</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>116840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>270509</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>16510</xdr:rowOff>
@@ -4525,6 +5973,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>34924</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>300990</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>181610</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50101E4F-0316-964E-5360-6AD65F3F1745}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4929,1237 +6413,2045 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+      <selection activeCell="H52" sqref="H20:H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="19.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2">
-        <f>$H$2*(1-EXP(-$H$3*A2))^2</f>
+      <c r="D2" s="6">
+        <f>B2</f>
         <v>0</v>
       </c>
-      <c r="F2">
-        <f>(E2-B2)^2</f>
+      <c r="E2" s="6">
+        <f>D2</f>
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="6">
+        <f>B2</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <f>B2</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2">
+        <f>$L$2*(1-EXP(-$L$3*A2))^2</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>(I2-B2)^2</f>
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
         <v>3</v>
       </c>
-      <c r="H2">
+      <c r="L2">
         <v>2221.7706877025917</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.35570308063309297</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="3">
         <v>0.2832059504711929</v>
       </c>
       <c r="D3" s="6">
+        <f t="shared" ref="D3:D29" si="0">B3</f>
+        <v>0.35570308063309297</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E29" si="1">D3</f>
+        <v>0.35570308063309297</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" ref="F3:F18" si="2">B3</f>
+        <v>0.35570308063309297</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G52" si="3">B3</f>
+        <v>0.35570308063309297</v>
+      </c>
+      <c r="H3" s="5">
         <f>1-(C3/B3)</f>
         <v>0.20381361340156823</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E52" si="0">$H$2*(1-EXP(-$H$3*A3))^2</f>
+      <c r="I3">
+        <f t="shared" ref="I3:I52" si="4">$L$2*(1-EXP(-$L$3*A3))^2</f>
         <v>3.3352895225504389</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F52" si="1">(E3-B3)^2</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J52" si="5">(I3-B3)^2</f>
         <v>8.8779353648576684</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="L3">
         <v>3.9515694715762335E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1.76</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="2">
         <v>1.76</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" ref="D4:D52" si="2">1-(C4/B4)</f>
+        <f t="shared" si="0"/>
+        <v>1.76</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="1"/>
+        <v>1.76</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="2"/>
+        <v>1.76</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="3"/>
+        <v>1.76</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" ref="H4:H52" si="6">1-(C4/B4)</f>
         <v>0</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
+      <c r="I4">
+        <f t="shared" si="4"/>
         <v>12.829260036603872</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="1"/>
+      <c r="J4">
+        <f t="shared" si="5"/>
         <v>122.52851775795556</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>5.28</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="2">
         <v>4.4000000000000004</v>
       </c>
       <c r="D5" s="6">
+        <f t="shared" si="0"/>
+        <v>5.28</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="1"/>
+        <v>5.28</v>
+      </c>
+      <c r="F5" s="6">
         <f t="shared" si="2"/>
+        <v>5.28</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="3"/>
+        <v>5.28</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" si="6"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
+      <c r="I5">
+        <f t="shared" si="4"/>
         <v>27.765480343110781</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
+      <c r="J5">
+        <f t="shared" si="5"/>
         <v>505.59682626042127</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>11</v>
       </c>
-      <c r="H5">
-        <f>SUM(F2:F52)</f>
+      <c r="L5">
+        <f>SUM(J2:J52)</f>
         <v>4548.1774113181564</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>22.88</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="2">
         <v>17.600000000000001</v>
       </c>
       <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>22.88</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="1"/>
+        <v>22.88</v>
+      </c>
+      <c r="F6" s="6">
         <f t="shared" si="2"/>
+        <v>22.88</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="3"/>
+        <v>22.88</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="6"/>
         <v>0.23076923076923073</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
+      <c r="I6">
+        <f t="shared" si="4"/>
         <v>47.491585981086061</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
+      <c r="J6">
+        <f t="shared" si="5"/>
         <v>605.73016450439195</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>52.8</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="2">
         <v>38.72</v>
       </c>
       <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>52.8</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="1"/>
+        <v>52.8</v>
+      </c>
+      <c r="F7" s="6">
         <f t="shared" si="2"/>
+        <v>52.8</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="3"/>
+        <v>52.8</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="6"/>
         <v>0.26666666666666661</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
+      <c r="I7">
+        <f t="shared" si="4"/>
         <v>71.414037902592668</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
+      <c r="J7">
+        <f t="shared" si="5"/>
         <v>346.48240703915656</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>96.8</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="2">
         <v>69.52</v>
       </c>
       <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>96.8</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="1"/>
+        <v>96.8</v>
+      </c>
+      <c r="F8" s="6">
         <f t="shared" si="2"/>
+        <v>96.8</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="3"/>
+        <v>96.8</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="6"/>
         <v>0.28181818181818186</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
+      <c r="I8">
+        <f t="shared" si="4"/>
         <v>98.993293881286888</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
+      <c r="J8">
+        <f t="shared" si="5"/>
         <v>4.8105380496905159</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>144.32</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="2">
         <v>106.48</v>
       </c>
       <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>144.32</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="1"/>
+        <v>144.32</v>
+      </c>
+      <c r="F9" s="6">
         <f t="shared" si="2"/>
+        <v>144.32</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="3"/>
+        <v>144.32</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="6"/>
         <v>0.26219512195121941</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
+      <c r="I9">
+        <f t="shared" si="4"/>
         <v>129.73936073141127</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
+      <c r="J9">
+        <f t="shared" si="5"/>
         <v>212.59504148071159</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>182.16</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="2">
         <v>135.52000000000001</v>
       </c>
       <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>182.16</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="1"/>
+        <v>182.16</v>
+      </c>
+      <c r="F10" s="6">
         <f t="shared" si="2"/>
+        <v>182.16</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="3"/>
+        <v>182.16</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="6"/>
         <v>0.25603864734299508</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
+      <c r="I10">
+        <f t="shared" si="4"/>
         <v>163.20769786162015</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
+      <c r="J10">
+        <f t="shared" si="5"/>
         <v>359.1897563444374</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>220.88</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="2">
         <v>156.64000000000001</v>
       </c>
       <c r="D11" s="6">
+        <f t="shared" si="0"/>
+        <v>220.88</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="1"/>
+        <v>220.88</v>
+      </c>
+      <c r="F11" s="6">
         <f t="shared" si="2"/>
+        <v>220.88</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="3"/>
+        <v>220.88</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" si="6"/>
         <v>0.29083665338645415</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
+      <c r="I11">
+        <f t="shared" si="4"/>
         <v>198.99544494870125</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
+      <c r="J11">
+        <f t="shared" si="5"/>
         <v>478.93374979332549</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>259.60000000000002</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="2">
         <v>178.64000000000001</v>
       </c>
       <c r="D12" s="6">
+        <f t="shared" si="0"/>
+        <v>259.60000000000002</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="1"/>
+        <v>259.60000000000002</v>
+      </c>
+      <c r="F12" s="6">
         <f t="shared" si="2"/>
+        <v>259.60000000000002</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" si="3"/>
+        <v>259.60000000000002</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="6"/>
         <v>0.31186440677966099</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
+      <c r="I12">
+        <f t="shared" si="4"/>
         <v>236.73794860433679</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
+      <c r="J12">
+        <f t="shared" si="5"/>
         <v>522.67339401794698</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>292.16000000000003</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="2">
         <v>200.64000000000001</v>
       </c>
       <c r="D13" s="6">
+        <f t="shared" si="0"/>
+        <v>292.16000000000003</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="1"/>
+        <v>292.16000000000003</v>
+      </c>
+      <c r="F13" s="6">
         <f t="shared" si="2"/>
+        <v>292.16000000000003</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="3"/>
+        <v>292.16000000000003</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="6"/>
         <v>0.31325301204819278</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
+      <c r="I13">
+        <f t="shared" si="4"/>
         <v>276.10556483668336</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
+      <c r="J13">
+        <f t="shared" si="5"/>
         <v>257.74488841313871</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>328.24</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="2">
         <v>213.84</v>
       </c>
       <c r="D14" s="6">
+        <f t="shared" si="0"/>
+        <v>328.24</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="1"/>
+        <v>328.24</v>
+      </c>
+      <c r="F14" s="6">
         <f t="shared" si="2"/>
+        <v>328.24</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="3"/>
+        <v>328.24</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="6"/>
         <v>0.34852546916890081</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
+      <c r="I14">
+        <f t="shared" si="4"/>
         <v>316.80071588987948</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
+      <c r="J14">
+        <f t="shared" si="5"/>
         <v>130.85722095205594</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>366.96</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="2">
         <v>227.92</v>
       </c>
       <c r="D15" s="6">
+        <f t="shared" si="0"/>
+        <v>366.96</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="1"/>
+        <v>366.96</v>
+      </c>
+      <c r="F15" s="6">
         <f t="shared" si="2"/>
+        <v>366.96</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="3"/>
+        <v>366.96</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="6"/>
         <v>0.37889688249400477</v>
       </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
+      <c r="I15">
+        <f t="shared" si="4"/>
         <v>358.5551816898473</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
+      <c r="J15">
+        <f t="shared" si="5"/>
         <v>70.640970826677702</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>408.32</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="2">
         <v>242.88</v>
       </c>
       <c r="D16" s="6">
+        <f t="shared" si="0"/>
+        <v>408.32</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="1"/>
+        <v>408.32</v>
+      </c>
+      <c r="F16" s="6">
         <f t="shared" si="2"/>
+        <v>408.32</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" si="3"/>
+        <v>408.32</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="6"/>
         <v>0.40517241379310343</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
+      <c r="I16">
+        <f t="shared" si="4"/>
         <v>401.12760764429066</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
+      <c r="J16">
+        <f t="shared" si="5"/>
         <v>51.730507798466007</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>449.68</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="2">
         <v>257.83999999999997</v>
       </c>
       <c r="D17" s="6">
+        <f t="shared" si="0"/>
+        <v>449.68</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="1"/>
+        <v>449.68</v>
+      </c>
+      <c r="F17" s="6">
         <f t="shared" si="2"/>
+        <v>449.68</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="3"/>
+        <v>449.68</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="6"/>
         <v>0.42661448140900204</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
+      <c r="I17">
+        <f t="shared" si="4"/>
         <v>444.30121194820737</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
+      <c r="J17">
+        <f t="shared" si="5"/>
         <v>28.931360906107258</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>492.8</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="2">
         <v>273.68</v>
       </c>
       <c r="D18" s="6">
+        <f t="shared" si="0"/>
+        <v>492.8</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="1"/>
+        <v>492.8</v>
+      </c>
+      <c r="F18" s="6">
         <f t="shared" si="2"/>
+        <v>492.8</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="3"/>
+        <v>492.8</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="6"/>
         <v>0.44464285714285712</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
+      <c r="I18">
+        <f t="shared" si="4"/>
         <v>487.88167684235907</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="1"/>
+      <c r="J18">
+        <f t="shared" si="5"/>
         <v>24.18990268298716</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>535.91999999999996</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="2">
         <v>289.52</v>
       </c>
       <c r="D19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>535.91999999999996</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="1"/>
+        <v>535.91999999999996</v>
+      </c>
+      <c r="F19" s="6">
+        <f>F18</f>
+        <v>492.8</v>
+      </c>
+      <c r="G19" s="6">
+        <f t="shared" si="3"/>
+        <v>535.91999999999996</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="6"/>
         <v>0.45977011494252873</v>
       </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
+      <c r="I19">
+        <f t="shared" si="4"/>
         <v>531.69520946916953</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="1"/>
+      <c r="J19">
+        <f t="shared" si="5"/>
         <v>17.848855029394489</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>579.04</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="2">
         <v>304.48</v>
       </c>
       <c r="D20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>579.04</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="1"/>
+        <v>579.04</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" ref="F20:F52" si="7">F19</f>
+        <v>492.8</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="3"/>
+        <v>579.04</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="6"/>
         <v>0.47416413373860178</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
+      <c r="I20">
+        <f t="shared" si="4"/>
         <v>575.58675907599195</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
+      <c r="J20">
+        <f t="shared" si="5"/>
         <v>11.924872879243724</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>622.16</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="2">
         <v>319.44</v>
       </c>
       <c r="D21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>622.16</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="1"/>
+        <v>622.16</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="3"/>
+        <v>622.16</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="6"/>
         <v>0.48656294200848649</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
+      <c r="I21">
+        <f t="shared" si="4"/>
         <v>619.41837833660145</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="1"/>
+      <c r="J21">
+        <f t="shared" si="5"/>
         <v>7.5164893452160602</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>664.4</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="2">
         <v>334.4</v>
       </c>
       <c r="D22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>664.4</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="1"/>
+        <v>664.4</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="3"/>
+        <v>664.4</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" si="6"/>
         <v>0.49668874172185429</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
+      <c r="I22">
+        <f t="shared" si="4"/>
         <v>663.06771750453436</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="1"/>
+      <c r="J22">
+        <f t="shared" si="5"/>
         <v>1.7749766477240994</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>706.64</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="2">
         <v>348.48</v>
       </c>
       <c r="D23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>706.64</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="1"/>
+        <v>706.64</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="3"/>
+        <v>706.64</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="6"/>
         <v>0.50684931506849318</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
+      <c r="I23">
+        <f t="shared" si="4"/>
         <v>706.42664098253658</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="1"/>
+      <c r="J23">
+        <f t="shared" si="5"/>
         <v>4.5522070332949E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>748</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="2">
         <v>363.44</v>
       </c>
       <c r="D24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>748</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="1"/>
+        <v>748</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="3"/>
+        <v>748</v>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" si="6"/>
         <v>0.51411764705882357</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
+      <c r="I24">
+        <f t="shared" si="4"/>
         <v>749.39995669631935</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="1"/>
+      <c r="J24">
+        <f t="shared" si="5"/>
         <v>1.9598787515693892</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>789.36</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="2">
         <v>377.52</v>
       </c>
       <c r="D25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>789.36</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" si="1"/>
+        <v>789.36</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="3"/>
+        <v>789.36</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="6"/>
         <v>0.52173913043478271</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
+      <c r="I25">
+        <f t="shared" si="4"/>
         <v>791.90424940322259</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="1"/>
+      <c r="J25">
+        <f t="shared" si="5"/>
         <v>6.4732050257984524</v>
       </c>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>830.72</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="2">
         <v>391.6</v>
       </c>
       <c r="D26" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>830.72</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="1"/>
+        <v>830.72</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="3"/>
+        <v>830.72</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" si="6"/>
         <v>0.52860169491525422</v>
       </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
+      <c r="I26">
+        <f t="shared" si="4"/>
         <v>833.86680975187892</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="1"/>
+      <c r="J26">
+        <f t="shared" si="5"/>
         <v>9.9024116145200871</v>
       </c>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>871.2</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="2">
         <v>406.56</v>
       </c>
       <c r="D27" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>871.2</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" si="1"/>
+        <v>871.2</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="3"/>
+        <v>871.2</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="6"/>
         <v>0.53333333333333344</v>
       </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
+      <c r="I27">
+        <f t="shared" si="4"/>
         <v>875.22465154194163</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="1"/>
+      <c r="J27">
+        <f t="shared" si="5"/>
         <v>16.197820034052739</v>
       </c>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>911.68</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="2">
         <v>419.76</v>
       </c>
       <c r="D28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>911.68</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="1"/>
+        <v>911.68</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="3"/>
+        <v>911.68</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="6"/>
         <v>0.53957528957528955</v>
       </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
+      <c r="I28">
+        <f t="shared" si="4"/>
         <v>915.92361021738816</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="1"/>
+      <c r="J28">
+        <f t="shared" si="5"/>
         <v>18.008227677121603</v>
       </c>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>951.28</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="2">
         <v>433.84</v>
       </c>
       <c r="D29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>951.28</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="1"/>
+        <v>951.28</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" si="3"/>
+        <v>951.28</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" si="6"/>
         <v>0.54394079555966701</v>
       </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
+      <c r="I29">
+        <f t="shared" si="4"/>
         <v>955.91751616651379</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="1"/>
+      <c r="J29">
+        <f t="shared" si="5"/>
         <v>21.506556194677032</v>
       </c>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>990.88</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="2">
         <v>447.92</v>
       </c>
       <c r="D30" s="6">
-        <f t="shared" si="2"/>
+        <f>C30</f>
+        <v>447.92</v>
+      </c>
+      <c r="E30" s="6">
+        <f>D30+B2</f>
+        <v>447.92</v>
+      </c>
+      <c r="F30" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="3"/>
+        <v>990.88</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" si="6"/>
         <v>0.54795737122557719</v>
       </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
+      <c r="I30">
+        <f t="shared" si="4"/>
         <v>995.16743689995258</v>
       </c>
-      <c r="F30">
-        <f t="shared" si="1"/>
+      <c r="J30">
+        <f t="shared" si="5"/>
         <v>18.382115171075</v>
       </c>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>1028.72</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="2">
         <v>461.12</v>
       </c>
       <c r="D31" s="6">
-        <f t="shared" si="2"/>
+        <f>D30-C$30/10</f>
+        <v>403.12800000000004</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" ref="E31:E52" si="8">D31+B3</f>
+        <v>403.48370308063312</v>
+      </c>
+      <c r="F31" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G31" s="6">
+        <f t="shared" si="3"/>
+        <v>1028.72</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="6"/>
         <v>0.5517536355859709</v>
       </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
+      <c r="I31">
+        <f t="shared" si="4"/>
         <v>1033.6409826380334</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="1"/>
+      <c r="J31">
+        <f t="shared" si="5"/>
         <v>24.216070123825819</v>
       </c>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>1066.56</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="2">
         <v>473.44</v>
       </c>
       <c r="D32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D32:D41" si="9">D31-C$30/10</f>
+        <v>358.33600000000001</v>
+      </c>
+      <c r="E32" s="6">
+        <f t="shared" si="8"/>
+        <v>360.096</v>
+      </c>
+      <c r="F32" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" si="3"/>
+        <v>1066.56</v>
+      </c>
+      <c r="H32" s="5">
+        <f t="shared" si="6"/>
         <v>0.55610561056105601</v>
       </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
+      <c r="I32">
+        <f t="shared" si="4"/>
         <v>1071.3116702634447</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="1"/>
+      <c r="J32">
+        <f t="shared" si="5"/>
         <v>22.578370292505515</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>1103.52</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="2">
         <v>486.64</v>
       </c>
       <c r="D33" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
+        <v>313.54399999999998</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="8"/>
+        <v>318.82399999999996</v>
+      </c>
+      <c r="F33" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G33" s="6">
+        <f t="shared" si="3"/>
+        <v>1103.52</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="6"/>
         <v>0.55901116427432218</v>
       </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
+      <c r="I33">
+        <f t="shared" si="4"/>
         <v>1108.1583409871894</v>
       </c>
-      <c r="F33">
-        <f t="shared" si="1"/>
+      <c r="J33">
+        <f t="shared" si="5"/>
         <v>21.514207113441088</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>1139.5999999999999</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="2">
         <v>498.96</v>
       </c>
       <c r="D34" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
+        <v>268.75199999999995</v>
+      </c>
+      <c r="E34" s="6">
+        <f t="shared" si="8"/>
+        <v>291.63199999999995</v>
+      </c>
+      <c r="F34" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G34" s="6">
+        <f t="shared" si="3"/>
+        <v>1139.5999999999999</v>
+      </c>
+      <c r="H34" s="5">
+        <f t="shared" si="6"/>
         <v>0.56216216216216219</v>
       </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
+      <c r="I34">
+        <f t="shared" si="4"/>
         <v>1144.164627437749</v>
       </c>
-      <c r="F34">
-        <f t="shared" si="1"/>
+      <c r="J34">
+        <f t="shared" si="5"/>
         <v>20.835823645451871</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>1173.92</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="2">
         <v>510.4</v>
       </c>
       <c r="D35" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
+        <v>223.95999999999995</v>
+      </c>
+      <c r="E35" s="6">
+        <f t="shared" si="8"/>
+        <v>276.75999999999993</v>
+      </c>
+      <c r="F35" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G35" s="6">
+        <f t="shared" si="3"/>
+        <v>1173.92</v>
+      </c>
+      <c r="H35" s="5">
+        <f t="shared" si="6"/>
         <v>0.56521739130434789</v>
       </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
+      <c r="I35">
+        <f t="shared" si="4"/>
         <v>1179.3184662174228</v>
       </c>
-      <c r="F35">
-        <f t="shared" si="1"/>
+      <c r="J35">
+        <f t="shared" si="5"/>
         <v>29.143437500654858</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>1208.24</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="2">
         <v>521.84</v>
       </c>
       <c r="D36" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
+        <v>179.16799999999995</v>
+      </c>
+      <c r="E36" s="6">
+        <f t="shared" si="8"/>
+        <v>275.96799999999996</v>
+      </c>
+      <c r="F36" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G36" s="6">
+        <f t="shared" si="3"/>
+        <v>1208.24</v>
+      </c>
+      <c r="H36" s="5">
+        <f t="shared" si="6"/>
         <v>0.56809905316824472</v>
       </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
+      <c r="I36">
+        <f t="shared" si="4"/>
         <v>1213.6116522782097</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="1"/>
+      <c r="J36">
+        <f t="shared" si="5"/>
         <v>28.854648197995402</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>1241.68</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="2">
         <v>533.28</v>
       </c>
       <c r="D37" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
+        <v>134.37599999999995</v>
+      </c>
+      <c r="E37" s="6">
+        <f t="shared" si="8"/>
+        <v>278.69599999999991</v>
+      </c>
+      <c r="F37" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G37" s="6">
+        <f t="shared" si="3"/>
+        <v>1241.68</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" si="6"/>
         <v>0.57051736357193483</v>
       </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
+      <c r="I37">
+        <f t="shared" si="4"/>
         <v>1247.0394317542336</v>
       </c>
-      <c r="F37">
-        <f t="shared" si="1"/>
+      <c r="J37">
+        <f t="shared" si="5"/>
         <v>28.723508728287261</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>1273.3599999999999</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="2">
         <v>544.72</v>
       </c>
       <c r="D38" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
+        <v>89.583999999999946</v>
+      </c>
+      <c r="E38" s="6">
+        <f t="shared" si="8"/>
+        <v>271.74399999999991</v>
+      </c>
+      <c r="F38" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G38" s="6">
+        <f t="shared" si="3"/>
+        <v>1273.3599999999999</v>
+      </c>
+      <c r="H38" s="5">
+        <f t="shared" si="6"/>
         <v>0.57221838286109183</v>
       </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
+      <c r="I38">
+        <f t="shared" si="4"/>
         <v>1279.6001301504357</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="1"/>
+      <c r="J38">
+        <f t="shared" si="5"/>
         <v>38.93922429437778</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>1305.04</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="2">
         <v>555.28</v>
       </c>
       <c r="D39" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
+        <v>44.791999999999945</v>
+      </c>
+      <c r="E39" s="6">
+        <f t="shared" si="8"/>
+        <v>265.67199999999991</v>
+      </c>
+      <c r="F39" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G39" s="6">
+        <f t="shared" si="3"/>
+        <v>1305.04</v>
+      </c>
+      <c r="H39" s="5">
+        <f t="shared" si="6"/>
         <v>0.57451112609575183</v>
       </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
+      <c r="I39">
+        <f t="shared" si="4"/>
         <v>1311.2948130297546</v>
       </c>
-      <c r="F39">
-        <f t="shared" si="1"/>
+      <c r="J39">
+        <f t="shared" si="5"/>
         <v>39.122686037187755</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>1336.72</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="2">
         <v>565.84</v>
       </c>
       <c r="D40" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
+        <v>-5.6843418860808015E-14</v>
+      </c>
+      <c r="E40" s="6">
+        <f t="shared" si="8"/>
+        <v>259.59999999999997</v>
+      </c>
+      <c r="F40" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G40" s="6">
+        <f t="shared" si="3"/>
+        <v>1336.72</v>
+      </c>
+      <c r="H40" s="5">
+        <f t="shared" si="6"/>
         <v>0.57669519420671489</v>
       </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
+      <c r="I40">
+        <f t="shared" si="4"/>
         <v>1342.1269765647878</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="1"/>
+      <c r="J40">
+        <f t="shared" si="5"/>
         <v>29.235395572164293</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>1366.64</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="2">
         <v>576.4</v>
       </c>
       <c r="D41" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="6">
+        <f t="shared" si="8"/>
+        <v>292.16000000000003</v>
+      </c>
+      <c r="F41" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G41" s="6">
+        <f t="shared" si="3"/>
+        <v>1366.64</v>
+      </c>
+      <c r="H41" s="5">
+        <f t="shared" si="6"/>
         <v>0.57823567289117839</v>
       </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
+      <c r="I41">
+        <f t="shared" si="4"/>
         <v>1372.1022655264685</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="1"/>
+      <c r="J41">
+        <f t="shared" si="5"/>
         <v>29.836344681645105</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>1396.56</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="2">
         <v>586.08000000000004</v>
       </c>
       <c r="D42" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="6">
+        <f t="shared" si="8"/>
+        <v>328.24</v>
+      </c>
+      <c r="F42" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G42" s="6">
+        <f t="shared" si="3"/>
+        <v>1396.56</v>
+      </c>
+      <c r="H42" s="5">
+        <f t="shared" si="6"/>
         <v>0.58034026465028354</v>
       </c>
-      <c r="E42">
-        <f t="shared" si="0"/>
+      <c r="I42">
+        <f t="shared" si="4"/>
         <v>1401.2282164728699</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="1"/>
+      <c r="J42">
+        <f t="shared" si="5"/>
         <v>21.79224503757456</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>1426.48</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43" s="2">
         <v>596.64</v>
       </c>
       <c r="D43" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="6">
+        <f t="shared" si="8"/>
+        <v>366.96</v>
+      </c>
+      <c r="F43" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G43" s="6">
+        <f t="shared" si="3"/>
+        <v>1426.48</v>
+      </c>
+      <c r="H43" s="5">
+        <f t="shared" si="6"/>
         <v>0.58173966687230105</v>
       </c>
-      <c r="E43">
-        <f t="shared" si="0"/>
+      <c r="I43">
+        <f t="shared" si="4"/>
         <v>1429.5140240771232</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="1"/>
+      <c r="J43">
+        <f t="shared" si="5"/>
         <v>9.205302100562978</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>1455.52</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44" s="2">
         <v>606.32000000000005</v>
       </c>
       <c r="D44" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="6">
+        <f t="shared" si="8"/>
+        <v>408.32</v>
+      </c>
+      <c r="F44" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G44" s="6">
+        <f t="shared" si="3"/>
+        <v>1455.52</v>
+      </c>
+      <c r="H44" s="5">
+        <f t="shared" si="6"/>
         <v>0.58343409915356714</v>
       </c>
-      <c r="E44">
-        <f t="shared" si="0"/>
+      <c r="I44">
+        <f t="shared" si="4"/>
         <v>1456.9703286957026</v>
       </c>
-      <c r="F44">
-        <f t="shared" si="1"/>
+      <c r="J44">
+        <f t="shared" si="5"/>
         <v>2.1034533255785139</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>1483.68</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="2">
         <v>616</v>
       </c>
       <c r="D45" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="6">
+        <f t="shared" si="8"/>
+        <v>449.68</v>
+      </c>
+      <c r="F45" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G45" s="6">
+        <f t="shared" si="3"/>
+        <v>1483.68</v>
+      </c>
+      <c r="H45" s="5">
+        <f t="shared" si="6"/>
         <v>0.58481613285883749</v>
       </c>
-      <c r="E45">
-        <f t="shared" si="0"/>
+      <c r="I45">
+        <f t="shared" si="4"/>
         <v>1483.6090234280678</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="1"/>
+      <c r="J45">
+        <f t="shared" si="5"/>
         <v>5.0376737632617918E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>1510.96</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="2">
         <v>624.79999999999995</v>
       </c>
       <c r="D46" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="6">
+        <f t="shared" si="8"/>
+        <v>492.8</v>
+      </c>
+      <c r="F46" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G46" s="6">
+        <f t="shared" si="3"/>
+        <v>1510.96</v>
+      </c>
+      <c r="H46" s="5">
+        <f t="shared" si="6"/>
         <v>0.58648806057076297</v>
       </c>
-      <c r="E46">
-        <f t="shared" si="0"/>
+      <c r="I46">
+        <f t="shared" si="4"/>
         <v>1509.4430790567667</v>
       </c>
-      <c r="F46">
-        <f t="shared" si="1"/>
+      <c r="J46">
+        <f t="shared" si="5"/>
         <v>2.3010491480199398</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>1537.36</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="2">
         <v>633.6</v>
       </c>
       <c r="D47" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="6">
+        <f t="shared" si="8"/>
+        <v>535.91999999999996</v>
+      </c>
+      <c r="F47" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G47" s="6">
+        <f t="shared" si="3"/>
+        <v>1537.36</v>
+      </c>
+      <c r="H47" s="5">
+        <f t="shared" si="6"/>
         <v>0.58786491127647389</v>
       </c>
-      <c r="E47">
-        <f t="shared" si="0"/>
+      <c r="I47">
+        <f t="shared" si="4"/>
         <v>1534.4863853845723</v>
       </c>
-      <c r="F47">
-        <f t="shared" si="1"/>
+      <c r="J47">
+        <f t="shared" si="5"/>
         <v>8.2576609579993505</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>1562.88</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="2">
         <v>642.4</v>
       </c>
       <c r="D48" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E48" s="6">
+        <f t="shared" si="8"/>
+        <v>579.04</v>
+      </c>
+      <c r="F48" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G48" s="6">
+        <f t="shared" si="3"/>
+        <v>1562.88</v>
+      </c>
+      <c r="H48" s="5">
+        <f t="shared" si="6"/>
         <v>0.588963963963964</v>
       </c>
-      <c r="E48">
-        <f t="shared" si="0"/>
+      <c r="I48">
+        <f t="shared" si="4"/>
         <v>1558.7536076027477</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="1"/>
+      <c r="J48">
+        <f t="shared" si="5"/>
         <v>17.027114216102429</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>1588.4</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49" s="2">
         <v>651.20000000000005</v>
       </c>
       <c r="D49" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E49" s="6">
+        <f t="shared" si="8"/>
+        <v>622.16</v>
+      </c>
+      <c r="F49" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G49" s="6">
+        <f t="shared" si="3"/>
+        <v>1588.4</v>
+      </c>
+      <c r="H49" s="5">
+        <f t="shared" si="6"/>
         <v>0.59002770083102485</v>
       </c>
-      <c r="E49">
-        <f t="shared" si="0"/>
+      <c r="I49">
+        <f t="shared" si="4"/>
         <v>1582.260056433006</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="1"/>
+      <c r="J49">
+        <f t="shared" si="5"/>
         <v>37.698907005872648</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>1612.16</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50" s="2">
         <v>659.12</v>
       </c>
       <c r="D50" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="6">
+        <f t="shared" si="8"/>
+        <v>664.4</v>
+      </c>
+      <c r="F50" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G50" s="6">
+        <f t="shared" si="3"/>
+        <v>1612.16</v>
+      </c>
+      <c r="H50" s="5">
+        <f t="shared" si="6"/>
         <v>0.59115720524017468</v>
       </c>
-      <c r="E50">
-        <f t="shared" si="0"/>
+      <c r="I50">
+        <f t="shared" si="4"/>
         <v>1605.0215708857238</v>
       </c>
-      <c r="F50">
-        <f t="shared" si="1"/>
+      <c r="J50">
+        <f t="shared" si="5"/>
         <v>50.957170219547201</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>1636.8</v>
       </c>
-      <c r="C51" s="9">
+      <c r="C51" s="2">
         <v>667.04</v>
       </c>
       <c r="D51" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E51" s="6">
+        <f t="shared" si="8"/>
+        <v>706.64</v>
+      </c>
+      <c r="F51" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G51" s="6">
+        <f t="shared" si="3"/>
+        <v>1636.8</v>
+      </c>
+      <c r="H51" s="5">
+        <f t="shared" si="6"/>
         <v>0.59247311827956994</v>
       </c>
-      <c r="E51">
-        <f t="shared" si="0"/>
+      <c r="I51">
+        <f t="shared" si="4"/>
         <v>1627.0544125692202</v>
       </c>
-      <c r="F51">
-        <f t="shared" si="1"/>
+      <c r="J51">
+        <f t="shared" si="5"/>
         <v>94.976474370972809</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="4">
         <v>1659.68</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="4">
         <v>674.96</v>
       </c>
       <c r="D52" s="6">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="6">
+        <f t="shared" si="8"/>
+        <v>748</v>
+      </c>
+      <c r="F52" s="6">
+        <f t="shared" si="7"/>
+        <v>492.8</v>
+      </c>
+      <c r="G52" s="6">
+        <f t="shared" si="3"/>
+        <v>1659.68</v>
+      </c>
+      <c r="H52" s="5">
+        <f t="shared" si="6"/>
         <v>0.59331919406150591</v>
       </c>
-      <c r="E52">
-        <f t="shared" si="0"/>
+      <c r="I52">
+        <f t="shared" si="4"/>
         <v>1648.3751705699922</v>
       </c>
-      <c r="F52">
-        <f t="shared" si="1"/>
+      <c r="J52">
+        <f t="shared" si="5"/>
         <v>127.79916844157241</v>
       </c>
     </row>

</xml_diff>